<commit_message>
revisi store db NAP4 financial personal
</commit_message>
<xml_diff>
--- a/Excel/4.1 ApplicationInquiryPersonal.xlsx
+++ b/Excel/4.1 ApplicationInquiryPersonal.xlsx
@@ -37,7 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Unexecuted</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -385,37 +392,125 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE1"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="3"/>
-    <col min="2" max="4" width="17" style="2"/>
-    <col min="5" max="23" width="17" style="3"/>
-    <col min="24" max="31" width="17" style="1"/>
-    <col min="32" max="16384" width="17" style="3"/>
+    <col min="1" max="1" width="17" style="3" collapsed="1"/>
+    <col min="2" max="4" width="17" style="2" collapsed="1"/>
+    <col min="5" max="23" width="17" style="3" collapsed="1"/>
+    <col min="24" max="31" width="17" style="1" collapsed="1"/>
+    <col min="32" max="16384" width="17" style="3" collapsed="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE1"/>
+  <dimension ref="B1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -423,13 +518,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="3"/>
-    <col min="2" max="4" width="17" style="2"/>
-    <col min="5" max="23" width="17" style="3"/>
-    <col min="24" max="31" width="17" style="1"/>
-    <col min="32" max="16384" width="17" style="3"/>
+    <col min="1" max="1" width="17" style="3" collapsed="1"/>
+    <col min="2" max="4" width="17" style="2" collapsed="1"/>
+    <col min="5" max="23" width="17" style="3" collapsed="1"/>
+    <col min="24" max="31" width="17" style="1" collapsed="1"/>
+    <col min="32" max="16384" width="17" style="3" collapsed="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>